<commit_message>
Done with revamping the locus names
</commit_message>
<xml_diff>
--- a/extras/Renaming-amplicons/ChinookFullPanelLociTable_May2024Updated.xlsx
+++ b/extras/Renaming-amplicons/ChinookFullPanelLociTable_May2024Updated.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriq/Documents/git-repos/california-chinook-microhaps/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eriq/Documents/git-repos/california-chinook-microhaps/extras/Renaming-amplicons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042437D-39EF-864F-9CF1-52F9BA52A920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0BD85-D5B5-524A-9B8C-18B5DB4D8524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5660" yWindow="760" windowWidth="27080" windowHeight="21580" xr2:uid="{E56130A1-82B1-034C-9FBF-E21DD198A6C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1481">
   <si>
     <t>ACTACAGGCACTCTCCCTGGCTAGAAGGGCAGGATAATAACAAACAAGAGATKATTTAAAGCCAGAGAAGTGATGGGGG</t>
   </si>
@@ -4476,6 +4476,12 @@
   </si>
   <si>
     <t>Waters et al. 2021</t>
+  </si>
+  <si>
+    <t>Thompson et al. 2019</t>
+  </si>
+  <si>
+    <t>Von Bargen et al. 2015 (MUST VERIFY)</t>
   </si>
 </sst>
 </file>
@@ -4949,8 +4955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575934F3-73D5-F049-89DB-6A73CBC8D927}">
   <dimension ref="A1:V205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I159" workbookViewId="0">
-      <selection activeCell="L209" sqref="L209"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J203" sqref="J203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11245,7 +11251,7 @@
         <v>1466</v>
       </c>
       <c r="L190" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
       <c r="M190"/>
     </row>
@@ -11344,7 +11350,7 @@
         <v>1466</v>
       </c>
       <c r="L193" s="13" t="s">
-        <v>1476</v>
+        <v>1479</v>
       </c>
       <c r="M193"/>
     </row>
@@ -11468,6 +11474,9 @@
       </c>
       <c r="K197" t="s">
         <v>1467</v>
+      </c>
+      <c r="L197" t="s">
+        <v>1480</v>
       </c>
       <c r="M197" t="s">
         <v>528</v>

</xml_diff>